<commit_message>
CEPA-313: add image question and fix update course
</commit_message>
<xml_diff>
--- a/public/file/sample.xlsx
+++ b/public/file/sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>statement</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Mệnh đề và tập hợp</t>
+  </si>
+  <si>
+    <t>imageUrl</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/a/ACg8ocIQfe1aUqsoSuK9TLzuzLVKQAArLvvNnHK2pqi8wQHw7A=s288-c-no</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,9 +419,10 @@
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="102" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +450,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -472,8 +482,11 @@
       <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>

</xml_diff>